<commit_message>
US Core Cond,Survey REdesign
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-us-core-encounter-diagnosis.xlsx
+++ b/docs/StructureDefinition-us-core-encounter-diagnosis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="353">
   <si>
     <t>Property</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>UsCoreEncounter Diagnosis</t>
+    <t>UsCoreEncounterDiagnosis</t>
   </si>
   <si>
     <t>Title</t>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-02-03</t>
+    <t>2022-03-17</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,181 +81,184 @@
     <t>Description</t>
   </si>
   <si>
+    <t>The US Core Encounter Diagnosis Profile is based upon the core FHIR Condition Resource and meets the  U.S. Core Data for Interoperability (USCDI) v2 'Encounter Diagnosis' requirements.  It defines constraints and extensions on the Condition resource for the minimal set of data to record, search, and fetch information about an encounter diagnosis.fhirVersion: 4.0.1</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>FHIR Version</t>
+  </si>
+  <si>
+    <t>4.0.1</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Base Definition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Condition</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Slice Name</t>
+  </si>
+  <si>
+    <t>Alias(s)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Must Support?</t>
+  </si>
+  <si>
+    <t>Is Modifier?</t>
+  </si>
+  <si>
+    <t>Is Summary?</t>
+  </si>
+  <si>
+    <t>Type(s)</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Meaning When Missing</t>
+  </si>
+  <si>
+    <t>Fixed Value</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Minimum Value</t>
+  </si>
+  <si>
+    <t>Maximum Value</t>
+  </si>
+  <si>
+    <t>Maximum Length</t>
+  </si>
+  <si>
+    <t>Binding Strength</t>
+  </si>
+  <si>
+    <t>Binding Description</t>
+  </si>
+  <si>
+    <t>Binding Value Set</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Slicing Discriminator</t>
+  </si>
+  <si>
+    <t>Slicing Description</t>
+  </si>
+  <si>
+    <t>Slicing Ordered</t>
+  </si>
+  <si>
+    <t>Slicing Rules</t>
+  </si>
+  <si>
+    <t>Base Path</t>
+  </si>
+  <si>
+    <t>Base Min</t>
+  </si>
+  <si>
+    <t>Base Max</t>
+  </si>
+  <si>
+    <t>Condition(s)</t>
+  </si>
+  <si>
+    <t>Constraint(s)</t>
+  </si>
+  <si>
+    <t>Mapping: Workflow Pattern</t>
+  </si>
+  <si>
+    <t>Mapping: SNOMED CT Concept Domain Binding</t>
+  </si>
+  <si>
+    <t>Mapping: HL7 v2 Mapping</t>
+  </si>
+  <si>
+    <t>Mapping: RIM Mapping</t>
+  </si>
+  <si>
+    <t>Mapping: FiveWs Pattern Mapping</t>
+  </si>
+  <si>
+    <t>Mapping: SNOMED CT Attribute Binding</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Detailed information about conditions, problems or diagnoses</t>
+  </si>
+  <si>
     <t>The US Core Encounter Diagnosis Profile is based upon the core FHIR Condition Resource and meets the  U.S. Core Data for Interoperability (USCDI) v2 'Encounter Diagnosis' requirements.  It defines constraints and extensions on the Condition resource for the minimal set of data to record, search, and fetch information about an encounter diagnosis.</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Copyright</t>
-  </si>
-  <si>
-    <t>FHIR Version</t>
-  </si>
-  <si>
-    <t>4.0.1</t>
-  </si>
-  <si>
-    <t>Kind</t>
-  </si>
-  <si>
-    <t>resource</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Base Definition</t>
-  </si>
-  <si>
-    <t>http://www.fhir.org/guides/healthedata1-sandbox/StructureDefinition/us-core-condition</t>
-  </si>
-  <si>
-    <t>Abstract</t>
-  </si>
-  <si>
-    <t>Derivation</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Slice Name</t>
-  </si>
-  <si>
-    <t>Alias(s)</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Must Support?</t>
-  </si>
-  <si>
-    <t>Is Modifier?</t>
-  </si>
-  <si>
-    <t>Is Summary?</t>
-  </si>
-  <si>
-    <t>Type(s)</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Meaning When Missing</t>
-  </si>
-  <si>
-    <t>Fixed Value</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
-    <t>Maximum Length</t>
-  </si>
-  <si>
-    <t>Binding Strength</t>
-  </si>
-  <si>
-    <t>Binding Description</t>
-  </si>
-  <si>
-    <t>Binding Value Set</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Slicing Discriminator</t>
-  </si>
-  <si>
-    <t>Slicing Description</t>
-  </si>
-  <si>
-    <t>Slicing Ordered</t>
-  </si>
-  <si>
-    <t>Slicing Rules</t>
-  </si>
-  <si>
-    <t>Base Path</t>
-  </si>
-  <si>
-    <t>Base Min</t>
-  </si>
-  <si>
-    <t>Base Max</t>
-  </si>
-  <si>
-    <t>Condition(s)</t>
-  </si>
-  <si>
-    <t>Constraint(s)</t>
-  </si>
-  <si>
-    <t>Mapping: Workflow Pattern</t>
-  </si>
-  <si>
-    <t>Mapping: SNOMED CT Concept Domain Binding</t>
-  </si>
-  <si>
-    <t>Mapping: HL7 v2 Mapping</t>
-  </si>
-  <si>
-    <t>Mapping: RIM Mapping</t>
-  </si>
-  <si>
-    <t>Mapping: FiveWs Pattern Mapping</t>
-  </si>
-  <si>
-    <t>Mapping: SNOMED CT Attribute Binding</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>Detailed information about an Encounter Diagnosis</t>
   </si>
   <si>
     <t>con-3:Condition.clinicalStatus SHALL be present if verificationStatus is not entered-in-error and category is problem-list-item {clinicalStatus.exists() or verificationStatus.coding.where(system='http://terminology.hl7.org/CodeSystem/condition-ver-status' and code = 'entered-in-error').exists() or category.select($this='problem-list-item').empty()}
@@ -641,9 +644,6 @@
     &lt;code value="encounter-diagnosis"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-condition-category</t>
   </si>
   <si>
     <t>Condition.severity</t>
@@ -1479,7 +1479,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="76.90625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="60.1328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
@@ -1654,7 +1654,7 @@
         <v>79</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1717,19 +1717,19 @@
         <v>76</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AL2" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AN2" t="s" s="2">
         <v>76</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1751,7 +1751,7 @@
         <v>77</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>76</v>
@@ -1760,19 +1760,19 @@
         <v>76</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
@@ -1822,13 +1822,13 @@
         <v>76</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>76</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1868,7 +1868,7 @@
         <v>77</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>76</v>
@@ -1877,16 +1877,16 @@
         <v>76</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1937,19 +1937,19 @@
         <v>76</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH4" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>76</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1983,28 +1983,28 @@
         <v>77</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -2054,19 +2054,19 @@
         <v>76</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>76</v>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -2100,7 +2100,7 @@
         <v>77</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>76</v>
@@ -2112,16 +2112,16 @@
         <v>76</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -2147,13 +2147,13 @@
         <v>76</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>76</v>
@@ -2171,19 +2171,19 @@
         <v>76</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>76</v>
@@ -2206,18 +2206,18 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>76</v>
@@ -2229,16 +2229,16 @@
         <v>76</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -2288,19 +2288,19 @@
         <v>76</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH7" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>76</v>
@@ -2312,7 +2312,7 @@
         <v>76</v>
       </c>
       <c r="AM7" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AN7" t="s" s="2">
         <v>76</v>
@@ -2323,11 +2323,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -2346,16 +2346,16 @@
         <v>76</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2405,7 +2405,7 @@
         <v>76</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>77</v>
@@ -2429,7 +2429,7 @@
         <v>76</v>
       </c>
       <c r="AM8" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN8" t="s" s="2">
         <v>76</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2463,13 +2463,13 @@
         <v>76</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2508,17 +2508,17 @@
         <v>76</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>77</v>
@@ -2530,7 +2530,7 @@
         <v>76</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>76</v>
@@ -2553,10 +2553,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>76</v>
@@ -2566,10 +2566,10 @@
         <v>77</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>76</v>
@@ -2578,16 +2578,16 @@
         <v>76</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -2637,7 +2637,7 @@
         <v>76</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>77</v>
@@ -2646,10 +2646,10 @@
         <v>78</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>76</v>
@@ -2672,11 +2672,11 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2689,25 +2689,25 @@
         <v>76</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>76</v>
@@ -2756,7 +2756,7 @@
         <v>76</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>77</v>
@@ -2768,7 +2768,7 @@
         <v>76</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>76</v>
@@ -2780,7 +2780,7 @@
         <v>76</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN11" t="s" s="2">
         <v>76</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2811,22 +2811,22 @@
         <v>76</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>76</v>
@@ -2875,7 +2875,7 @@
         <v>76</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>77</v>
@@ -2887,10 +2887,10 @@
         <v>76</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>76</v>
@@ -2899,10 +2899,10 @@
         <v>76</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>76</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2921,28 +2921,28 @@
         <v>77</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2968,11 +2968,11 @@
         <v>76</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>76</v>
@@ -2990,34 +2990,34 @@
         <v>76</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>76</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3036,28 +3036,28 @@
         <v>77</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3083,11 +3083,11 @@
         <v>76</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>76</v>
@@ -3105,42 +3105,42 @@
         <v>76</v>
       </c>
       <c r="AE14" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="AI14" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="AK14" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AL14" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AM14" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AN14" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AF14" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="AM14" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="AN14" t="s" s="2">
-        <v>172</v>
-      </c>
       <c r="AO14" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3148,13 +3148,13 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>76</v>
@@ -3163,16 +3163,16 @@
         <v>76</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3198,29 +3198,29 @@
         <v>76</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AB15" s="2"/>
       <c r="AC15" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>77</v>
@@ -3229,25 +3229,25 @@
         <v>78</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>76</v>
@@ -3255,23 +3255,23 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>76</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>76</v>
@@ -3280,16 +3280,16 @@
         <v>76</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3300,7 +3300,7 @@
         <v>76</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S16" t="s" s="2">
         <v>76</v>
@@ -3315,11 +3315,13 @@
         <v>76</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="X16" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>186</v>
+      </c>
       <c r="Y16" t="s" s="2">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>76</v>
@@ -3337,7 +3339,7 @@
         <v>76</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>77</v>
@@ -3349,22 +3351,22 @@
         <v>76</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>76</v>
@@ -3383,7 +3385,7 @@
         <v>77</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>76</v>
@@ -3395,7 +3397,7 @@
         <v>76</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K17" t="s" s="2">
         <v>200</v>
@@ -3430,7 +3432,7 @@
         <v>76</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X17" t="s" s="2">
         <v>201</v>
@@ -3460,13 +3462,13 @@
         <v>77</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>76</v>
@@ -3497,22 +3499,22 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K18" t="s" s="2">
         <v>211</v>
@@ -3547,7 +3549,7 @@
         <v>76</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="X18" t="s" s="2">
         <v>214</v>
@@ -3577,13 +3579,13 @@
         <v>77</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>216</v>
@@ -3626,10 +3628,10 @@
         <v>76</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K19" t="s" s="2">
         <v>223</v>
@@ -3700,7 +3702,7 @@
         <v>76</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>76</v>
@@ -3731,19 +3733,19 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J20" t="s" s="2">
         <v>234</v>
@@ -3808,16 +3810,16 @@
         <v>232</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>238</v>
@@ -3851,16 +3853,16 @@
         <v>77</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J21" t="s" s="2">
         <v>243</v>
@@ -3928,13 +3930,13 @@
         <v>77</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>247</v>
@@ -3968,16 +3970,16 @@
         <v>77</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>252</v>
@@ -4045,13 +4047,13 @@
         <v>77</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>256</v>
@@ -4085,10 +4087,10 @@
         <v>77</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>76</v>
@@ -4162,13 +4164,13 @@
         <v>77</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>264</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>76</v>
@@ -4202,16 +4204,16 @@
         <v>77</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J24" t="s" s="2">
         <v>268</v>
@@ -4277,13 +4279,13 @@
         <v>77</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>76</v>
@@ -4317,7 +4319,7 @@
         <v>77</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>76</v>
@@ -4326,7 +4328,7 @@
         <v>76</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J25" t="s" s="2">
         <v>275</v>
@@ -4392,13 +4394,13 @@
         <v>77</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>76</v>
@@ -4432,7 +4434,7 @@
         <v>77</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>76</v>
@@ -4441,7 +4443,7 @@
         <v>76</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J26" t="s" s="2">
         <v>275</v>
@@ -4507,13 +4509,13 @@
         <v>77</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>76</v>
@@ -4662,7 +4664,7 @@
         <v>77</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>76</v>
@@ -4674,7 +4676,7 @@
         <v>76</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>293</v>
@@ -4737,7 +4739,7 @@
         <v>77</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>76</v>
@@ -4770,7 +4772,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4789,7 +4791,7 @@
         <v>76</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>298</v>
@@ -4798,7 +4800,7 @@
         <v>299</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4860,7 +4862,7 @@
         <v>76</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>76</v>
@@ -4900,13 +4902,13 @@
         <v>76</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K30" t="s" s="2">
         <v>303</v>
@@ -4915,10 +4917,10 @@
         <v>304</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>76</v>
@@ -4979,7 +4981,7 @@
         <v>76</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>76</v>
@@ -4991,7 +4993,7 @@
         <v>76</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>76</v>
@@ -5013,7 +5015,7 @@
         <v>77</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>76</v>
@@ -5025,7 +5027,7 @@
         <v>76</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K31" t="s" s="2">
         <v>307</v>
@@ -5088,13 +5090,13 @@
         <v>77</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>311</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>76</v>
@@ -5103,7 +5105,7 @@
         <v>312</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>219</v>
@@ -5209,7 +5211,7 @@
         <v>311</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>76</v>
@@ -5243,7 +5245,7 @@
         <v>77</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>76</v>
@@ -5255,7 +5257,7 @@
         <v>76</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>319</v>
@@ -5318,13 +5320,13 @@
         <v>77</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>76</v>
@@ -5475,7 +5477,7 @@
         <v>77</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>76</v>
@@ -5487,7 +5489,7 @@
         <v>76</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>293</v>
@@ -5550,7 +5552,7 @@
         <v>77</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>76</v>
@@ -5583,7 +5585,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5602,7 +5604,7 @@
         <v>76</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K36" t="s" s="2">
         <v>298</v>
@@ -5611,7 +5613,7 @@
         <v>299</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5673,7 +5675,7 @@
         <v>76</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>76</v>
@@ -5713,13 +5715,13 @@
         <v>76</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K37" t="s" s="2">
         <v>303</v>
@@ -5728,10 +5730,10 @@
         <v>304</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>76</v>
@@ -5792,7 +5794,7 @@
         <v>76</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>76</v>
@@ -5804,7 +5806,7 @@
         <v>76</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>76</v>
@@ -5835,10 +5837,10 @@
         <v>76</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K38" t="s" s="2">
         <v>334</v>
@@ -5907,13 +5909,13 @@
         <v>338</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>339</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>76</v>
@@ -5950,7 +5952,7 @@
         <v>76</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J39" t="s" s="2">
         <v>343</v>
@@ -6022,7 +6024,7 @@
         <v>338</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>76</v>
@@ -6137,7 +6139,7 @@
         <v>76</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>350</v>

</xml_diff>